<commit_message>
Added New Milestone plan!.xlsx and working on a UI for the client + UDP
</commit_message>
<xml_diff>
--- a/Planning/New Milestone plan!.xlsx
+++ b/Planning/New Milestone plan!.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\James\Documents\DTU IT\Git Rep\DTU-IT\Planning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\DTU\GIT Repository\DTU IT\DTU-IT\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14376" windowHeight="5940"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="5940"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="71">
   <si>
     <t>TrainServer:</t>
   </si>
@@ -129,13 +129,121 @@
   </si>
   <si>
     <t>The new graph is distributed around to train and bus servers</t>
+  </si>
+  <si>
+    <t>Charge a user</t>
+  </si>
+  <si>
+    <t>Trainservers will request a user to be charged in the user database</t>
+  </si>
+  <si>
+    <t>An rmi call from the train server requests a user object to charge. The server searches for an cached user object in a user array</t>
+  </si>
+  <si>
+    <t>if the object exists, the RMI handler will charge that user object</t>
+  </si>
+  <si>
+    <t>if it doesn't exist the object is made from the database and put into the array. Maybe use a map to guarantee uniqueness.</t>
+  </si>
+  <si>
+    <t>A call to charge a user is stored in a concurrent array</t>
+  </si>
+  <si>
+    <t>A single looping thread reads the array and updates the database with the charges.</t>
+  </si>
+  <si>
+    <t>Scenario A: RMI - Advantage: shows RMI in use</t>
+  </si>
+  <si>
+    <t>Scenario B: Producer/Consumer - Advantage: is simple and stabile</t>
+  </si>
+  <si>
+    <t>Manage databases</t>
+  </si>
+  <si>
+    <t>Creating, deleting, updating, and getting entries in database tables</t>
+  </si>
+  <si>
+    <t>A single entry to each database that handles connection and takes in query strings</t>
+  </si>
+  <si>
+    <t>A function for addingUser</t>
+  </si>
+  <si>
+    <t>A function for deletingUser</t>
+  </si>
+  <si>
+    <t>A function for chargingUser</t>
+  </si>
+  <si>
+    <t>a function for UpdatingUser</t>
+  </si>
+  <si>
+    <t>a function for getting user</t>
+  </si>
+  <si>
+    <t>a function for getting graph</t>
+  </si>
+  <si>
+    <t>Assigned to</t>
+  </si>
+  <si>
+    <t>Workload (hours)</t>
+  </si>
+  <si>
+    <t>Deadline</t>
+  </si>
+  <si>
+    <t>James</t>
+  </si>
+  <si>
+    <t>Lukas</t>
+  </si>
+  <si>
+    <t>Sudhir</t>
+  </si>
+  <si>
+    <t>UI</t>
+  </si>
+  <si>
+    <t>An suggestion for an interface on the client "PDA" showing status to a conductor</t>
+  </si>
+  <si>
+    <t>Designing the layout</t>
+  </si>
+  <si>
+    <t>Listening for logged in status</t>
+  </si>
+  <si>
+    <t>Get journey screen with destination field and button.</t>
+  </si>
+  <si>
+    <t>Calculate charge</t>
+  </si>
+  <si>
+    <t>calculating what to charge a user when that user leaves the train/bus</t>
+  </si>
+  <si>
+    <t>Finding the dearest zone a passenger has been to.</t>
+  </si>
+  <si>
+    <t>finding the start zone</t>
+  </si>
+  <si>
+    <t>Calculating the cost per zone times the number of zones between start and destination</t>
+  </si>
+  <si>
+    <t>Current progress</t>
+  </si>
+  <si>
+    <t>Remaining</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -151,16 +259,43 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -168,11 +303,38 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -182,17 +344,44 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="3" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="3" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="Calculation" xfId="2" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="3" builtinId="24"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -470,184 +659,970 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H35"/>
+  <dimension ref="B2:I63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="43.77734375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" style="6" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="8"/>
+    <col min="9" max="9" width="10.42578125" style="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C2" t="s">
+    <row r="2" spans="2:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="C2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="2:8" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="2" t="s">
+      <c r="D2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="7">
+        <f>F4+F11+F18</f>
+        <v>76</v>
+      </c>
+      <c r="G3" s="6"/>
+      <c r="H3" s="8">
+        <f>AVERAGE(H4,H11,H18)</f>
+        <v>0.12777777777777777</v>
+      </c>
+      <c r="I3" s="12">
+        <f>I4+I11+I18</f>
+        <v>47.3</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" s="3" customFormat="1" ht="28.9" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-    </row>
-    <row r="4" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="D4" s="1" t="s">
+      <c r="F4" s="4">
+        <f>SUM(F5:F9)</f>
+        <v>52</v>
+      </c>
+      <c r="H4" s="9">
+        <f>AVERAGE(H5:H9)</f>
+        <v>0.3</v>
+      </c>
+      <c r="I4" s="13">
+        <f>SUM(I5:I9)</f>
+        <v>23.8</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="D5" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="D5" s="1" t="s">
+      <c r="E5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F5" s="6">
+        <v>2</v>
+      </c>
+      <c r="H5" s="8">
+        <v>0</v>
+      </c>
+      <c r="I5" s="11">
+        <f>F5*(1-H5)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D6" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="D6" s="1" t="s">
+      <c r="E6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F6" s="6">
+        <v>16</v>
+      </c>
+      <c r="H6" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="I6" s="11">
+        <f t="shared" ref="I6:I63" si="0">F6*(1-H6)</f>
+        <v>3.1999999999999993</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="D7" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="D7" s="1" t="s">
+      <c r="E7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F7" s="6">
+        <v>22</v>
+      </c>
+      <c r="H7" s="8">
+        <v>0.7</v>
+      </c>
+      <c r="I7" s="11">
+        <f t="shared" si="0"/>
+        <v>6.6000000000000014</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="D8" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="D8" s="1" t="s">
+      <c r="E8" t="s">
+        <v>56</v>
+      </c>
+      <c r="F8" s="6">
+        <v>10</v>
+      </c>
+      <c r="H8" s="8">
+        <v>0</v>
+      </c>
+      <c r="I8" s="11">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D9" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C10" s="2" t="s">
+      <c r="E9" t="s">
+        <v>56</v>
+      </c>
+      <c r="F9" s="6">
+        <v>2</v>
+      </c>
+      <c r="H9" s="8">
+        <v>0</v>
+      </c>
+      <c r="I9" s="11">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="C11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="D11" s="1" t="s">
+      <c r="F11" s="4">
+        <f>SUM(F12:F17)</f>
         <v>12</v>
       </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H11" s="9">
+        <f>AVERAGE(H12:H17)</f>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="I11" s="13">
+        <f>SUM(I12:I17)</f>
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" t="s">
+        <v>56</v>
+      </c>
+      <c r="F12" s="6">
+        <v>1</v>
+      </c>
+      <c r="H12" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="I12" s="11">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="D13" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="13" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="D13" s="1" t="s">
+      <c r="E13" t="s">
+        <v>56</v>
+      </c>
+      <c r="F13" s="6">
+        <v>2</v>
+      </c>
+      <c r="H13" s="8">
+        <v>0</v>
+      </c>
+      <c r="I13" s="11">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="D14" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="14" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="D14" s="1" t="s">
+      <c r="E14" t="s">
+        <v>56</v>
+      </c>
+      <c r="F14" s="6">
+        <v>3</v>
+      </c>
+      <c r="H14" s="8">
+        <v>0</v>
+      </c>
+      <c r="I14" s="11">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="D15" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="D15" s="1" t="s">
+      <c r="E15" t="s">
+        <v>56</v>
+      </c>
+      <c r="F15" s="6">
+        <v>3</v>
+      </c>
+      <c r="H15" s="8">
+        <v>0</v>
+      </c>
+      <c r="I15" s="11">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D16" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="16" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="D16" s="1" t="s">
+      <c r="E16" t="s">
+        <v>56</v>
+      </c>
+      <c r="F16" s="6">
+        <v>1</v>
+      </c>
+      <c r="H16" s="8">
+        <v>0</v>
+      </c>
+      <c r="I16" s="11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="D17" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B19" t="s">
+      <c r="E17" t="s">
+        <v>56</v>
+      </c>
+      <c r="F17" s="6">
+        <v>2</v>
+      </c>
+      <c r="H17" s="8">
+        <v>0</v>
+      </c>
+      <c r="I17" s="11">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="C18" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F18" s="4">
+        <f>SUM(F19:F21)</f>
+        <v>12</v>
+      </c>
+      <c r="H18" s="9">
+        <f>AVERAGE(H19:H21)</f>
+        <v>0</v>
+      </c>
+      <c r="I18" s="13">
+        <f>SUM(I19:I21)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="D19" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E19" t="s">
+        <v>56</v>
+      </c>
+      <c r="F19" s="6">
+        <v>4</v>
+      </c>
+      <c r="H19" s="8">
+        <v>0</v>
+      </c>
+      <c r="I19" s="11">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D20" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E20" t="s">
+        <v>56</v>
+      </c>
+      <c r="F20" s="6">
+        <v>4</v>
+      </c>
+      <c r="H20" s="8">
+        <v>0</v>
+      </c>
+      <c r="I20" s="11">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="D21" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E21" t="s">
+        <v>56</v>
+      </c>
+      <c r="F21" s="6">
+        <v>4</v>
+      </c>
+      <c r="H21" s="8">
+        <v>0</v>
+      </c>
+      <c r="I21" s="11">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C20" s="5" t="s">
+      <c r="F24" s="10">
+        <f>F25+F30+F34</f>
+        <v>23</v>
+      </c>
+      <c r="H24" s="8">
+        <f>AVERAGE(H25,H30,H34)</f>
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="I24" s="12">
+        <f>I25+I30+I34</f>
+        <v>17.5</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" s="3" customFormat="1" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C25" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D25" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="21" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="D21" s="1" t="s">
+      <c r="F25" s="4">
+        <f>SUM(F26:F28)</f>
+        <v>6</v>
+      </c>
+      <c r="H25" s="9">
+        <f>AVERAGE(H26:H28)</f>
+        <v>0.43333333333333335</v>
+      </c>
+      <c r="I25" s="13">
+        <f>SUM(I26:I28)</f>
+        <v>2.5999999999999996</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="D26" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="22" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="D22" s="1" t="s">
+      <c r="E26" t="s">
+        <v>56</v>
+      </c>
+      <c r="F26" s="6">
+        <v>3</v>
+      </c>
+      <c r="H26" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="I26" s="11">
+        <f t="shared" si="0"/>
+        <v>0.59999999999999987</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="D27" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="23" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="D23" s="1" t="s">
+      <c r="E27" t="s">
+        <v>56</v>
+      </c>
+      <c r="F27" s="6">
+        <v>2</v>
+      </c>
+      <c r="H27" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="I27" s="11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="D28" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C25" s="2" t="s">
+      <c r="E28" t="s">
+        <v>56</v>
+      </c>
+      <c r="F28" s="6">
+        <v>1</v>
+      </c>
+      <c r="H28" s="8">
+        <v>0</v>
+      </c>
+      <c r="I28" s="11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="C30" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D30" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="D26" s="1" t="s">
+      <c r="F30" s="4">
+        <f>SUM(F31:F32)</f>
+        <v>8</v>
+      </c>
+      <c r="H30" s="9">
+        <f>AVERAGE(H31:H32)</f>
+        <v>0</v>
+      </c>
+      <c r="I30" s="13">
+        <f>SUM(I31:I32)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D31" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="27" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="D27" s="1" t="s">
+      <c r="F31" s="6">
+        <v>2</v>
+      </c>
+      <c r="H31" s="8">
+        <v>0</v>
+      </c>
+      <c r="I31" s="11">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="D32" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B30" t="s">
+      <c r="F32" s="6">
+        <v>6</v>
+      </c>
+      <c r="H32" s="8">
+        <v>0</v>
+      </c>
+      <c r="I32" s="11">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="C34" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F34" s="4">
+        <f>SUM(F35:F37)</f>
+        <v>9</v>
+      </c>
+      <c r="H34" s="9">
+        <f>AVERAGE(H35:H37)</f>
+        <v>0.23333333333333331</v>
+      </c>
+      <c r="I34" s="13">
+        <f>SUM(I35:I37)</f>
+        <v>6.9</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D35" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E35" t="s">
+        <v>56</v>
+      </c>
+      <c r="F35" s="6">
+        <v>3</v>
+      </c>
+      <c r="H35" s="8">
+        <v>0.7</v>
+      </c>
+      <c r="I35" s="11">
+        <f t="shared" si="0"/>
+        <v>0.90000000000000013</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D36" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E36" t="s">
+        <v>56</v>
+      </c>
+      <c r="F36" s="6">
+        <v>2</v>
+      </c>
+      <c r="H36" s="8">
+        <v>0</v>
+      </c>
+      <c r="I36" s="11">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="D37" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E37" t="s">
+        <v>56</v>
+      </c>
+      <c r="F37" s="6">
+        <v>4</v>
+      </c>
+      <c r="H37" s="8">
+        <v>0</v>
+      </c>
+      <c r="I37" s="11">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="31" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C31" s="4" t="s">
+      <c r="F40" s="10">
+        <f>F41+F48+F52+F56</f>
+        <v>68</v>
+      </c>
+      <c r="H40" s="8">
+        <f>AVERAGE(H41,H48,H52,H56)</f>
+        <v>0</v>
+      </c>
+      <c r="I40" s="12">
+        <f>I41+I48+I52+I56</f>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9" s="3" customFormat="1" ht="45.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C41" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="D41" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="D32" s="1" t="s">
+      <c r="F41" s="4">
+        <f>SUM(F42:F45)</f>
+        <v>23</v>
+      </c>
+      <c r="H41" s="9">
+        <f>AVERAGE(H42:H45)</f>
+        <v>0</v>
+      </c>
+      <c r="I41" s="13">
+        <f>SUM(I42:I45)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="D42" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="4:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="D33" s="1" t="s">
+      <c r="F42" s="6">
+        <v>3</v>
+      </c>
+      <c r="H42" s="8">
+        <v>0</v>
+      </c>
+      <c r="I42" s="11">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="D43" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="4:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="D34" s="1" t="s">
+      <c r="F43" s="6">
+        <v>2</v>
+      </c>
+      <c r="H43" s="8">
+        <v>0</v>
+      </c>
+      <c r="I43" s="11">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="2:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="D44" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="35" spans="4:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="D35" s="1" t="s">
+      <c r="F44" s="6">
+        <v>16</v>
+      </c>
+      <c r="H44" s="8">
+        <v>0</v>
+      </c>
+      <c r="I44" s="11">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="45" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="D45" s="1" t="s">
         <v>34</v>
+      </c>
+      <c r="F45" s="6">
+        <v>2</v>
+      </c>
+      <c r="H45" s="8">
+        <v>0</v>
+      </c>
+      <c r="I45" s="11">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="2:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="C47" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F47" s="4"/>
+      <c r="H47" s="9"/>
+      <c r="I47" s="13"/>
+    </row>
+    <row r="48" spans="2:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D48" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F48" s="4">
+        <f>SUM(F49:F51)</f>
+        <v>21</v>
+      </c>
+      <c r="H48" s="9">
+        <f>AVERAGE(H49:H51)</f>
+        <v>0</v>
+      </c>
+      <c r="I48" s="13">
+        <f>SUM(I49:I51)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="49" spans="3:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="D49" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E49" t="s">
+        <v>57</v>
+      </c>
+      <c r="F49" s="6">
+        <v>15</v>
+      </c>
+      <c r="H49" s="8">
+        <v>0</v>
+      </c>
+      <c r="I49" s="11">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="50" spans="3:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="D50" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E50" t="s">
+        <v>57</v>
+      </c>
+      <c r="F50" s="6">
+        <v>2</v>
+      </c>
+      <c r="H50" s="8">
+        <v>0</v>
+      </c>
+      <c r="I50" s="11">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="3:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="D51" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E51" t="s">
+        <v>57</v>
+      </c>
+      <c r="F51" s="6">
+        <v>4</v>
+      </c>
+      <c r="H51" s="8">
+        <v>0</v>
+      </c>
+      <c r="I51" s="11">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="3:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="D52" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F52" s="4">
+        <f>SUM(F53:F54)</f>
+        <v>6</v>
+      </c>
+      <c r="H52" s="9">
+        <f>AVERAGE(H53:H54)</f>
+        <v>0</v>
+      </c>
+      <c r="I52" s="13">
+        <f>SUM(I53:I54)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="53" spans="3:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="D53" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E53" t="s">
+        <v>57</v>
+      </c>
+      <c r="F53" s="6">
+        <v>2</v>
+      </c>
+      <c r="H53" s="8">
+        <v>0</v>
+      </c>
+      <c r="I53" s="11">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="3:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="D54" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E54" t="s">
+        <v>57</v>
+      </c>
+      <c r="F54" s="6">
+        <v>4</v>
+      </c>
+      <c r="H54" s="8">
+        <v>0</v>
+      </c>
+      <c r="I54" s="11">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="3:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="C56" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F56" s="4">
+        <f>SUM(F57:F63)</f>
+        <v>18</v>
+      </c>
+      <c r="H56" s="9">
+        <f>AVERAGE(H57:H63)</f>
+        <v>0</v>
+      </c>
+      <c r="I56" s="13">
+        <f>SUM(I57:I63)</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="57" spans="3:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="D57" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E57" t="s">
+        <v>56</v>
+      </c>
+      <c r="F57" s="6">
+        <v>1</v>
+      </c>
+      <c r="H57" s="8">
+        <v>0</v>
+      </c>
+      <c r="I57" s="11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="D58" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E58" t="s">
+        <v>58</v>
+      </c>
+      <c r="F58" s="6">
+        <v>3</v>
+      </c>
+      <c r="H58" s="8">
+        <v>0</v>
+      </c>
+      <c r="I58" s="11">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="D59" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E59" t="s">
+        <v>58</v>
+      </c>
+      <c r="F59" s="6">
+        <v>2</v>
+      </c>
+      <c r="H59" s="8">
+        <v>0</v>
+      </c>
+      <c r="I59" s="11">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="D60" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E60" t="s">
+        <v>57</v>
+      </c>
+      <c r="F60" s="6">
+        <v>4</v>
+      </c>
+      <c r="H60" s="8">
+        <v>0</v>
+      </c>
+      <c r="I60" s="11">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="61" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="D61" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E61" t="s">
+        <v>58</v>
+      </c>
+      <c r="F61" s="6">
+        <v>4</v>
+      </c>
+      <c r="H61" s="8">
+        <v>0</v>
+      </c>
+      <c r="I61" s="11">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="D62" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E62" t="s">
+        <v>58</v>
+      </c>
+      <c r="F62" s="6">
+        <v>2</v>
+      </c>
+      <c r="H62" s="8">
+        <v>0</v>
+      </c>
+      <c r="I62" s="11">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="D63" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E63" t="s">
+        <v>56</v>
+      </c>
+      <c r="F63" s="6">
+        <v>2</v>
+      </c>
+      <c r="H63" s="8">
+        <v>0</v>
+      </c>
+      <c r="I63" s="11">
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed from UDP to TCP for client connection for faster tests
</commit_message>
<xml_diff>
--- a/Planning/New Milestone plan!.xlsx
+++ b/Planning/New Milestone plan!.xlsx
@@ -662,7 +662,7 @@
   <dimension ref="B2:I63"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -713,11 +713,11 @@
       <c r="G3" s="6"/>
       <c r="H3" s="8">
         <f>AVERAGE(H4,H11,H18)</f>
-        <v>0.12777777777777777</v>
+        <v>0.16111111111111112</v>
       </c>
       <c r="I3" s="12">
         <f>I4+I11+I18</f>
-        <v>47.3</v>
+        <v>42.3</v>
       </c>
     </row>
     <row r="4" spans="2:9" s="3" customFormat="1" ht="28.9" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -733,11 +733,11 @@
       </c>
       <c r="H4" s="9">
         <f>AVERAGE(H5:H9)</f>
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="I4" s="13">
         <f>SUM(I5:I9)</f>
-        <v>23.8</v>
+        <v>18.8</v>
       </c>
     </row>
     <row r="5" spans="2:9" ht="30" x14ac:dyDescent="0.25">
@@ -805,11 +805,11 @@
         <v>10</v>
       </c>
       <c r="H8" s="8">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I8" s="11">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Modified Client to handle TCP and started on UDP
</commit_message>
<xml_diff>
--- a/Planning/New Milestone plan!.xlsx
+++ b/Planning/New Milestone plan!.xlsx
@@ -295,7 +295,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -327,6 +327,45 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -334,47 +373,67 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="3" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="3" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="4" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="5" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -659,974 +718,1129 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:I63"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A2:H63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="G56" sqref="G56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="43.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10" style="6" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="8"/>
-    <col min="9" max="9" width="10.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" style="4" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="5"/>
+    <col min="8" max="8" width="10.42578125" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="C2" s="4" t="s">
+    <row r="2" spans="1:8" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="4" t="s">
+      <c r="C2" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="E2" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="F2" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="G2" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="H2" s="10" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="7">
-        <f>F4+F11+F18</f>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="11"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="13">
+        <f>E4+E11+E18</f>
         <v>76</v>
       </c>
-      <c r="G3" s="6"/>
-      <c r="H3" s="8">
-        <f>AVERAGE(H4,H11,H18)</f>
+      <c r="F3" s="11"/>
+      <c r="G3" s="14">
+        <f>AVERAGE(G4,G11,G18)</f>
         <v>0.16111111111111112</v>
       </c>
-      <c r="I3" s="12">
-        <f>I4+I11+I18</f>
+      <c r="H3" s="15">
+        <f>H4+H11+H18</f>
         <v>42.3</v>
       </c>
     </row>
-    <row r="4" spans="2:9" s="3" customFormat="1" ht="28.9" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="2" t="s">
+    <row r="4" spans="1:8" s="2" customFormat="1" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="C4" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="4">
-        <f>SUM(F5:F9)</f>
+      <c r="D4" s="17"/>
+      <c r="E4" s="7">
+        <f>SUM(E5:E9)</f>
         <v>52</v>
       </c>
-      <c r="H4" s="9">
-        <f>AVERAGE(H5:H9)</f>
+      <c r="F4" s="17"/>
+      <c r="G4" s="18">
+        <f>AVERAGE(G5:G9)</f>
         <v>0.4</v>
       </c>
-      <c r="I4" s="13">
-        <f>SUM(I5:I9)</f>
+      <c r="H4" s="10">
+        <f>SUM(H5:H9)</f>
         <v>18.8</v>
       </c>
     </row>
-    <row r="5" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="D5" s="1" t="s">
+    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B5" s="19"/>
+      <c r="C5" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="E5" t="s">
-        <v>56</v>
-      </c>
-      <c r="F5" s="6">
-        <v>2</v>
-      </c>
-      <c r="H5" s="8">
-        <v>0</v>
-      </c>
-      <c r="I5" s="11">
-        <f>F5*(1-H5)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D6" s="1" t="s">
+      <c r="D5" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="E5" s="11">
+        <v>2</v>
+      </c>
+      <c r="F5" s="19"/>
+      <c r="G5" s="14">
+        <v>0</v>
+      </c>
+      <c r="H5" s="20">
+        <f>E5*(1-G5)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="19"/>
+      <c r="C6" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="E6" t="s">
-        <v>56</v>
-      </c>
-      <c r="F6" s="6">
+      <c r="D6" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="E6" s="11">
         <v>16</v>
       </c>
-      <c r="H6" s="8">
+      <c r="F6" s="19"/>
+      <c r="G6" s="14">
         <v>0.8</v>
       </c>
-      <c r="I6" s="11">
-        <f t="shared" ref="I6:I63" si="0">F6*(1-H6)</f>
+      <c r="H6" s="20">
+        <f t="shared" ref="H6:H63" si="0">E6*(1-G6)</f>
         <v>3.1999999999999993</v>
       </c>
     </row>
-    <row r="7" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="D7" s="1" t="s">
+    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B7" s="19"/>
+      <c r="C7" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F7" s="6">
+      <c r="D7" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="E7" s="11">
         <v>22</v>
       </c>
-      <c r="H7" s="8">
+      <c r="F7" s="19"/>
+      <c r="G7" s="14">
         <v>0.7</v>
       </c>
-      <c r="I7" s="11">
+      <c r="H7" s="20">
         <f t="shared" si="0"/>
         <v>6.6000000000000014</v>
       </c>
     </row>
-    <row r="8" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="D8" s="1" t="s">
+    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B8" s="19"/>
+      <c r="C8" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="E8" t="s">
-        <v>56</v>
-      </c>
-      <c r="F8" s="6">
+      <c r="D8" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="E8" s="11">
         <v>10</v>
       </c>
-      <c r="H8" s="8">
+      <c r="F8" s="19"/>
+      <c r="G8" s="14">
         <v>0.5</v>
       </c>
-      <c r="I8" s="11">
+      <c r="H8" s="20">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D9" s="1" t="s">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="19"/>
+      <c r="C9" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E9" t="s">
-        <v>56</v>
-      </c>
-      <c r="F9" s="6">
-        <v>2</v>
-      </c>
-      <c r="H9" s="8">
-        <v>0</v>
-      </c>
-      <c r="I9" s="11">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="2:9" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="C11" s="2" t="s">
+      <c r="D9" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9" s="11">
+        <v>2</v>
+      </c>
+      <c r="F9" s="19"/>
+      <c r="G9" s="14">
+        <v>0</v>
+      </c>
+      <c r="H9" s="20">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="19"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="20"/>
+    </row>
+    <row r="11" spans="1:8" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="B11" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="C11" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="4">
-        <f>SUM(F12:F17)</f>
+      <c r="D11" s="17"/>
+      <c r="E11" s="7">
+        <f>SUM(E12:E17)</f>
         <v>12</v>
       </c>
-      <c r="H11" s="9">
-        <f>AVERAGE(H12:H17)</f>
+      <c r="F11" s="17"/>
+      <c r="G11" s="18">
+        <f>AVERAGE(G12:G17)</f>
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="I11" s="13">
-        <f>SUM(I12:I17)</f>
+      <c r="H11" s="10">
+        <f>SUM(H12:H17)</f>
         <v>11.5</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D12" s="1" t="s">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="19"/>
+      <c r="C12" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E12" t="s">
-        <v>56</v>
-      </c>
-      <c r="F12" s="6">
+      <c r="D12" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="E12" s="11">
         <v>1</v>
       </c>
-      <c r="H12" s="8">
+      <c r="F12" s="19"/>
+      <c r="G12" s="14">
         <v>0.5</v>
       </c>
-      <c r="I12" s="11">
+      <c r="H12" s="20">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
     </row>
-    <row r="13" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="D13" s="1" t="s">
+    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B13" s="19"/>
+      <c r="C13" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="E13" t="s">
-        <v>56</v>
-      </c>
-      <c r="F13" s="6">
-        <v>2</v>
-      </c>
-      <c r="H13" s="8">
-        <v>0</v>
-      </c>
-      <c r="I13" s="11">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="D14" s="1" t="s">
+      <c r="D13" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="E13" s="11">
+        <v>2</v>
+      </c>
+      <c r="F13" s="19"/>
+      <c r="G13" s="14">
+        <v>0</v>
+      </c>
+      <c r="H13" s="20">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B14" s="19"/>
+      <c r="C14" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="E14" t="s">
-        <v>56</v>
-      </c>
-      <c r="F14" s="6">
+      <c r="D14" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="E14" s="11">
         <v>3</v>
       </c>
-      <c r="H14" s="8">
-        <v>0</v>
-      </c>
-      <c r="I14" s="11">
+      <c r="F14" s="19"/>
+      <c r="G14" s="14">
+        <v>0</v>
+      </c>
+      <c r="H14" s="20">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="D15" s="1" t="s">
+    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B15" s="19"/>
+      <c r="C15" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="E15" t="s">
-        <v>56</v>
-      </c>
-      <c r="F15" s="6">
+      <c r="D15" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="E15" s="11">
         <v>3</v>
       </c>
-      <c r="H15" s="8">
-        <v>0</v>
-      </c>
-      <c r="I15" s="11">
+      <c r="F15" s="19"/>
+      <c r="G15" s="14">
+        <v>0</v>
+      </c>
+      <c r="H15" s="20">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D16" s="1" t="s">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="19"/>
+      <c r="C16" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E16" t="s">
-        <v>56</v>
-      </c>
-      <c r="F16" s="6">
+      <c r="D16" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="E16" s="11">
         <v>1</v>
       </c>
-      <c r="H16" s="8">
-        <v>0</v>
-      </c>
-      <c r="I16" s="11">
+      <c r="F16" s="19"/>
+      <c r="G16" s="14">
+        <v>0</v>
+      </c>
+      <c r="H16" s="20">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="D17" s="1" t="s">
+    <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B17" s="19"/>
+      <c r="C17" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E17" t="s">
-        <v>56</v>
-      </c>
-      <c r="F17" s="6">
-        <v>2</v>
-      </c>
-      <c r="H17" s="8">
-        <v>0</v>
-      </c>
-      <c r="I17" s="11">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="2:9" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="C18" s="4" t="s">
+      <c r="D17" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="E17" s="11">
+        <v>2</v>
+      </c>
+      <c r="F17" s="19"/>
+      <c r="G17" s="14">
+        <v>0</v>
+      </c>
+      <c r="H17" s="20">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B18" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="C18" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="F18" s="4">
-        <f>SUM(F19:F21)</f>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7">
+        <f>SUM(E19:E21)</f>
         <v>12</v>
       </c>
-      <c r="H18" s="9">
-        <f>AVERAGE(H19:H21)</f>
-        <v>0</v>
-      </c>
-      <c r="I18" s="13">
-        <f>SUM(I19:I21)</f>
+      <c r="F18" s="7"/>
+      <c r="G18" s="18">
+        <f>AVERAGE(G19:G21)</f>
+        <v>0</v>
+      </c>
+      <c r="H18" s="10">
+        <f>SUM(H19:H21)</f>
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="D19" s="1" t="s">
+    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B19" s="19"/>
+      <c r="C19" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="E19" t="s">
-        <v>56</v>
-      </c>
-      <c r="F19" s="6">
+      <c r="D19" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="E19" s="11">
         <v>4</v>
       </c>
-      <c r="H19" s="8">
-        <v>0</v>
-      </c>
-      <c r="I19" s="11">
+      <c r="F19" s="19"/>
+      <c r="G19" s="14">
+        <v>0</v>
+      </c>
+      <c r="H19" s="20">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D20" s="1" t="s">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="19"/>
+      <c r="C20" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="E20" t="s">
-        <v>56</v>
-      </c>
-      <c r="F20" s="6">
+      <c r="D20" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="E20" s="11">
         <v>4</v>
       </c>
-      <c r="H20" s="8">
-        <v>0</v>
-      </c>
-      <c r="I20" s="11">
+      <c r="F20" s="19"/>
+      <c r="G20" s="14">
+        <v>0</v>
+      </c>
+      <c r="H20" s="20">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="D21" s="1" t="s">
+    <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B21" s="19"/>
+      <c r="C21" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="E21" t="s">
-        <v>56</v>
-      </c>
-      <c r="F21" s="6">
+      <c r="D21" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="E21" s="11">
         <v>4</v>
       </c>
-      <c r="H21" s="8">
-        <v>0</v>
-      </c>
-      <c r="I21" s="11">
+      <c r="F21" s="19"/>
+      <c r="G21" s="14">
+        <v>0</v>
+      </c>
+      <c r="H21" s="20">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" t="s">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>18</v>
       </c>
-      <c r="F24" s="10">
-        <f>F25+F30+F34</f>
+      <c r="E24" s="21">
+        <f>E25+E30+E34</f>
         <v>23</v>
       </c>
-      <c r="H24" s="8">
-        <f>AVERAGE(H25,H30,H34)</f>
+      <c r="G24" s="5">
+        <f>AVERAGE(G25,G30,G34)</f>
         <v>0.22222222222222221</v>
       </c>
-      <c r="I24" s="12">
-        <f>I25+I30+I34</f>
+      <c r="H24" s="22">
+        <f>H25+H30+H34</f>
         <v>17.5</v>
       </c>
     </row>
-    <row r="25" spans="2:9" s="3" customFormat="1" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C25" s="4" t="s">
+    <row r="25" spans="1:8" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B25" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="C25" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="F25" s="4">
-        <f>SUM(F26:F28)</f>
+      <c r="D25" s="17"/>
+      <c r="E25" s="7">
+        <f>SUM(E26:E28)</f>
         <v>6</v>
       </c>
-      <c r="H25" s="9">
-        <f>AVERAGE(H26:H28)</f>
+      <c r="F25" s="17"/>
+      <c r="G25" s="18">
+        <f>AVERAGE(G26:G28)</f>
         <v>0.43333333333333335</v>
       </c>
-      <c r="I25" s="13">
-        <f>SUM(I26:I28)</f>
+      <c r="H25" s="10">
+        <f>SUM(H26:H28)</f>
         <v>2.5999999999999996</v>
       </c>
     </row>
-    <row r="26" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="D26" s="1" t="s">
+    <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B26" s="19"/>
+      <c r="C26" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="E26" t="s">
-        <v>56</v>
-      </c>
-      <c r="F26" s="6">
+      <c r="D26" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="E26" s="11">
         <v>3</v>
       </c>
-      <c r="H26" s="8">
+      <c r="F26" s="19"/>
+      <c r="G26" s="14">
         <v>0.8</v>
       </c>
-      <c r="I26" s="11">
+      <c r="H26" s="20">
         <f t="shared" si="0"/>
         <v>0.59999999999999987</v>
       </c>
     </row>
-    <row r="27" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="D27" s="1" t="s">
+    <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B27" s="19"/>
+      <c r="C27" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="E27" t="s">
-        <v>56</v>
-      </c>
-      <c r="F27" s="6">
-        <v>2</v>
-      </c>
-      <c r="H27" s="8">
+      <c r="D27" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="E27" s="11">
+        <v>2</v>
+      </c>
+      <c r="F27" s="19"/>
+      <c r="G27" s="14">
         <v>0.5</v>
       </c>
-      <c r="I27" s="11">
+      <c r="H27" s="20">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="D28" s="1" t="s">
+    <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B28" s="19"/>
+      <c r="C28" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="E28" t="s">
-        <v>56</v>
-      </c>
-      <c r="F28" s="6">
+      <c r="D28" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="E28" s="11">
         <v>1</v>
       </c>
-      <c r="H28" s="8">
-        <v>0</v>
-      </c>
-      <c r="I28" s="11">
+      <c r="F28" s="19"/>
+      <c r="G28" s="14">
+        <v>0</v>
+      </c>
+      <c r="H28" s="20">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="2:9" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="C30" s="2" t="s">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="19"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="20"/>
+    </row>
+    <row r="30" spans="1:8" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="B30" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="C30" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="F30" s="4">
-        <f>SUM(F31:F32)</f>
+      <c r="D30" s="17"/>
+      <c r="E30" s="7">
+        <f>SUM(E31:E32)</f>
         <v>8</v>
       </c>
-      <c r="H30" s="9">
-        <f>AVERAGE(H31:H32)</f>
-        <v>0</v>
-      </c>
-      <c r="I30" s="13">
-        <f>SUM(I31:I32)</f>
+      <c r="F30" s="17"/>
+      <c r="G30" s="18">
+        <f>AVERAGE(G31:G32)</f>
+        <v>0</v>
+      </c>
+      <c r="H30" s="10">
+        <f>SUM(H31:H32)</f>
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D31" s="1" t="s">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B31" s="19"/>
+      <c r="C31" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="F31" s="6">
-        <v>2</v>
-      </c>
-      <c r="H31" s="8">
-        <v>0</v>
-      </c>
-      <c r="I31" s="11">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="2:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="D32" s="1" t="s">
+      <c r="D31" s="19"/>
+      <c r="E31" s="11">
+        <v>2</v>
+      </c>
+      <c r="F31" s="19"/>
+      <c r="G31" s="14">
+        <v>0</v>
+      </c>
+      <c r="H31" s="20">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="B32" s="19"/>
+      <c r="C32" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="F32" s="6">
+      <c r="D32" s="19"/>
+      <c r="E32" s="11">
         <v>6</v>
       </c>
-      <c r="H32" s="8">
-        <v>0</v>
-      </c>
-      <c r="I32" s="11">
+      <c r="F32" s="19"/>
+      <c r="G32" s="14">
+        <v>0</v>
+      </c>
+      <c r="H32" s="20">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="2:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="C34" s="3" t="s">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B33" s="19"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="19"/>
+      <c r="G33" s="14"/>
+      <c r="H33" s="20"/>
+    </row>
+    <row r="34" spans="1:8" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B34" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="C34" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="F34" s="4">
-        <f>SUM(F35:F37)</f>
+      <c r="D34" s="17"/>
+      <c r="E34" s="7">
+        <f>SUM(E35:E37)</f>
         <v>9</v>
       </c>
-      <c r="H34" s="9">
-        <f>AVERAGE(H35:H37)</f>
+      <c r="F34" s="17"/>
+      <c r="G34" s="18">
+        <f>AVERAGE(G35:G37)</f>
         <v>0.23333333333333331</v>
       </c>
-      <c r="I34" s="13">
-        <f>SUM(I35:I37)</f>
+      <c r="H34" s="10">
+        <f>SUM(H35:H37)</f>
         <v>6.9</v>
       </c>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D35" s="1" t="s">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B35" s="19"/>
+      <c r="C35" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="E35" t="s">
-        <v>56</v>
-      </c>
-      <c r="F35" s="6">
+      <c r="D35" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="E35" s="11">
         <v>3</v>
       </c>
-      <c r="H35" s="8">
+      <c r="F35" s="19"/>
+      <c r="G35" s="14">
         <v>0.7</v>
       </c>
-      <c r="I35" s="11">
+      <c r="H35" s="20">
         <f t="shared" si="0"/>
         <v>0.90000000000000013</v>
       </c>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D36" s="1" t="s">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B36" s="19"/>
+      <c r="C36" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="E36" t="s">
-        <v>56</v>
-      </c>
-      <c r="F36" s="6">
-        <v>2</v>
-      </c>
-      <c r="H36" s="8">
-        <v>0</v>
-      </c>
-      <c r="I36" s="11">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="D37" s="1" t="s">
+      <c r="D36" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="E36" s="11">
+        <v>2</v>
+      </c>
+      <c r="F36" s="19"/>
+      <c r="G36" s="14">
+        <v>0</v>
+      </c>
+      <c r="H36" s="20">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B37" s="19"/>
+      <c r="C37" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="E37" t="s">
-        <v>56</v>
-      </c>
-      <c r="F37" s="6">
+      <c r="D37" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="E37" s="11">
         <v>4</v>
       </c>
-      <c r="H37" s="8">
-        <v>0</v>
-      </c>
-      <c r="I37" s="11">
+      <c r="F37" s="19"/>
+      <c r="G37" s="14">
+        <v>0</v>
+      </c>
+      <c r="H37" s="20">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B40" t="s">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>28</v>
       </c>
-      <c r="F40" s="10">
-        <f>F41+F48+F52+F56</f>
+      <c r="E40" s="21">
+        <f>E41+E48+E52+E56</f>
         <v>68</v>
       </c>
-      <c r="H40" s="8">
-        <f>AVERAGE(H41,H48,H52,H56)</f>
-        <v>0</v>
-      </c>
-      <c r="I40" s="12">
-        <f>I41+I48+I52+I56</f>
-        <v>68</v>
-      </c>
-    </row>
-    <row r="41" spans="2:9" s="3" customFormat="1" ht="45.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C41" s="2" t="s">
+      <c r="G40" s="5">
+        <f>AVERAGE(G41,G48,G52,G56)</f>
+        <v>5.7142857142857148E-2</v>
+      </c>
+      <c r="H40" s="22">
+        <f>H41+H48+H52+H56</f>
+        <v>65.8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="B41" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="C41" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="F41" s="4">
-        <f>SUM(F42:F45)</f>
+      <c r="D41" s="17"/>
+      <c r="E41" s="7">
+        <f>SUM(E42:E45)</f>
         <v>23</v>
       </c>
-      <c r="H41" s="9">
-        <f>AVERAGE(H42:H45)</f>
-        <v>0</v>
-      </c>
-      <c r="I41" s="13">
-        <f>SUM(I42:I45)</f>
+      <c r="F41" s="17"/>
+      <c r="G41" s="18">
+        <f>AVERAGE(G42:G45)</f>
+        <v>0</v>
+      </c>
+      <c r="H41" s="10">
+        <f>SUM(H42:H45)</f>
         <v>23</v>
       </c>
     </row>
-    <row r="42" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="D42" s="1" t="s">
+    <row r="42" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B42" s="19"/>
+      <c r="C42" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="F42" s="6">
+      <c r="D42" s="19"/>
+      <c r="E42" s="11">
         <v>3</v>
       </c>
-      <c r="H42" s="8">
-        <v>0</v>
-      </c>
-      <c r="I42" s="11">
+      <c r="F42" s="19"/>
+      <c r="G42" s="14">
+        <v>0</v>
+      </c>
+      <c r="H42" s="20">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="D43" s="1" t="s">
+    <row r="43" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B43" s="19"/>
+      <c r="C43" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="F43" s="6">
-        <v>2</v>
-      </c>
-      <c r="H43" s="8">
-        <v>0</v>
-      </c>
-      <c r="I43" s="11">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="44" spans="2:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="D44" s="1" t="s">
+      <c r="D43" s="19"/>
+      <c r="E43" s="11">
+        <v>2</v>
+      </c>
+      <c r="F43" s="19"/>
+      <c r="G43" s="14">
+        <v>0</v>
+      </c>
+      <c r="H43" s="20">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="B44" s="19"/>
+      <c r="C44" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F44" s="6">
+      <c r="D44" s="19"/>
+      <c r="E44" s="11">
         <v>16</v>
       </c>
-      <c r="H44" s="8">
-        <v>0</v>
-      </c>
-      <c r="I44" s="11">
+      <c r="F44" s="19"/>
+      <c r="G44" s="14">
+        <v>0</v>
+      </c>
+      <c r="H44" s="20">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
     </row>
-    <row r="45" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="D45" s="1" t="s">
+    <row r="45" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B45" s="19"/>
+      <c r="C45" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="F45" s="6">
-        <v>2</v>
-      </c>
-      <c r="H45" s="8">
-        <v>0</v>
-      </c>
-      <c r="I45" s="11">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="47" spans="2:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="C47" s="3" t="s">
+      <c r="D45" s="19"/>
+      <c r="E45" s="11">
+        <v>2</v>
+      </c>
+      <c r="F45" s="19"/>
+      <c r="G45" s="14">
+        <v>0</v>
+      </c>
+      <c r="H45" s="20">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B46" s="19"/>
+      <c r="C46" s="12"/>
+      <c r="D46" s="19"/>
+      <c r="E46" s="11"/>
+      <c r="F46" s="19"/>
+      <c r="G46" s="14"/>
+      <c r="H46" s="20"/>
+    </row>
+    <row r="47" spans="1:8" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B47" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="D47" s="2" t="s">
+      <c r="C47" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="F47" s="4"/>
-      <c r="H47" s="9"/>
-      <c r="I47" s="13"/>
-    </row>
-    <row r="48" spans="2:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D48" s="2" t="s">
+      <c r="D47" s="17"/>
+      <c r="E47" s="7"/>
+      <c r="F47" s="17"/>
+      <c r="G47" s="18"/>
+      <c r="H47" s="10"/>
+    </row>
+    <row r="48" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="17"/>
+      <c r="C48" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="F48" s="4">
-        <f>SUM(F49:F51)</f>
+      <c r="D48" s="17"/>
+      <c r="E48" s="7">
+        <f>SUM(E49:E51)</f>
         <v>21</v>
       </c>
-      <c r="H48" s="9">
-        <f>AVERAGE(H49:H51)</f>
-        <v>0</v>
-      </c>
-      <c r="I48" s="13">
-        <f>SUM(I49:I51)</f>
+      <c r="F48" s="17"/>
+      <c r="G48" s="18">
+        <f>AVERAGE(G49:G51)</f>
+        <v>0</v>
+      </c>
+      <c r="H48" s="10">
+        <f>SUM(H49:H51)</f>
         <v>21</v>
       </c>
     </row>
-    <row r="49" spans="3:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="D49" s="1" t="s">
+    <row r="49" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="B49" s="19"/>
+      <c r="C49" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="E49" t="s">
+      <c r="D49" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="F49" s="6">
+      <c r="E49" s="11">
         <v>15</v>
       </c>
-      <c r="H49" s="8">
-        <v>0</v>
-      </c>
-      <c r="I49" s="11">
+      <c r="F49" s="19"/>
+      <c r="G49" s="14">
+        <v>0</v>
+      </c>
+      <c r="H49" s="20">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
     </row>
-    <row r="50" spans="3:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="D50" s="1" t="s">
+    <row r="50" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B50" s="19"/>
+      <c r="C50" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="E50" t="s">
+      <c r="D50" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="F50" s="6">
-        <v>2</v>
-      </c>
-      <c r="H50" s="8">
-        <v>0</v>
-      </c>
-      <c r="I50" s="11">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="51" spans="3:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="D51" s="1" t="s">
+      <c r="E50" s="11">
+        <v>2</v>
+      </c>
+      <c r="F50" s="19"/>
+      <c r="G50" s="14">
+        <v>0</v>
+      </c>
+      <c r="H50" s="20">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="B51" s="19"/>
+      <c r="C51" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="E51" t="s">
+      <c r="D51" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="F51" s="6">
+      <c r="E51" s="11">
         <v>4</v>
       </c>
-      <c r="H51" s="8">
-        <v>0</v>
-      </c>
-      <c r="I51" s="11">
+      <c r="F51" s="19"/>
+      <c r="G51" s="14">
+        <v>0</v>
+      </c>
+      <c r="H51" s="20">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="3:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="D52" s="2" t="s">
+    <row r="52" spans="2:8" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B52" s="17"/>
+      <c r="C52" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="F52" s="4">
-        <f>SUM(F53:F54)</f>
+      <c r="D52" s="17"/>
+      <c r="E52" s="7">
+        <f>SUM(E53:E54)</f>
         <v>6</v>
       </c>
-      <c r="H52" s="9">
-        <f>AVERAGE(H53:H54)</f>
-        <v>0</v>
-      </c>
-      <c r="I52" s="13">
-        <f>SUM(I53:I54)</f>
+      <c r="F52" s="17"/>
+      <c r="G52" s="18">
+        <f>AVERAGE(G53:G54)</f>
+        <v>0</v>
+      </c>
+      <c r="H52" s="10">
+        <f>SUM(H53:H54)</f>
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="3:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="D53" s="1" t="s">
+    <row r="53" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B53" s="19"/>
+      <c r="C53" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="E53" t="s">
+      <c r="D53" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="F53" s="6">
-        <v>2</v>
-      </c>
-      <c r="H53" s="8">
-        <v>0</v>
-      </c>
-      <c r="I53" s="11">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="54" spans="3:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="D54" s="1" t="s">
+      <c r="E53" s="11">
+        <v>2</v>
+      </c>
+      <c r="F53" s="19"/>
+      <c r="G53" s="14">
+        <v>0</v>
+      </c>
+      <c r="H53" s="20">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B54" s="19"/>
+      <c r="C54" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="E54" t="s">
+      <c r="D54" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="F54" s="6">
+      <c r="E54" s="11">
         <v>4</v>
       </c>
-      <c r="H54" s="8">
-        <v>0</v>
-      </c>
-      <c r="I54" s="11">
+      <c r="F54" s="19"/>
+      <c r="G54" s="14">
+        <v>0</v>
+      </c>
+      <c r="H54" s="20">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="3:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="C56" s="3" t="s">
+    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B55" s="19"/>
+      <c r="C55" s="12"/>
+      <c r="D55" s="19"/>
+      <c r="E55" s="11"/>
+      <c r="F55" s="19"/>
+      <c r="G55" s="14"/>
+      <c r="H55" s="20"/>
+    </row>
+    <row r="56" spans="2:8" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B56" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="D56" s="2" t="s">
+      <c r="C56" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="F56" s="4">
-        <f>SUM(F57:F63)</f>
+      <c r="D56" s="17"/>
+      <c r="E56" s="7">
+        <f>SUM(E57:E63)</f>
         <v>18</v>
       </c>
-      <c r="H56" s="9">
-        <f>AVERAGE(H57:H63)</f>
-        <v>0</v>
-      </c>
-      <c r="I56" s="13">
-        <f>SUM(I57:I63)</f>
-        <v>18</v>
-      </c>
-    </row>
-    <row r="57" spans="3:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="D57" s="1" t="s">
+      <c r="F56" s="17"/>
+      <c r="G56" s="18">
+        <f>AVERAGE(G57:G63)</f>
+        <v>0.22857142857142859</v>
+      </c>
+      <c r="H56" s="10">
+        <f>SUM(H57:H63)</f>
+        <v>15.8</v>
+      </c>
+    </row>
+    <row r="57" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B57" s="19"/>
+      <c r="C57" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="E57" t="s">
-        <v>56</v>
-      </c>
-      <c r="F57" s="6">
+      <c r="D57" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="E57" s="11">
         <v>1</v>
       </c>
-      <c r="H57" s="8">
-        <v>0</v>
-      </c>
-      <c r="I57" s="11">
-        <f t="shared" si="0"/>
+      <c r="F57" s="19"/>
+      <c r="G57" s="14">
         <v>1</v>
       </c>
-    </row>
-    <row r="58" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="D58" s="1" t="s">
+      <c r="H57" s="20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B58" s="19"/>
+      <c r="C58" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="E58" t="s">
+      <c r="D58" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="F58" s="6">
+      <c r="E58" s="11">
         <v>3</v>
       </c>
-      <c r="H58" s="8">
-        <v>0</v>
-      </c>
-      <c r="I58" s="11">
+      <c r="F58" s="19"/>
+      <c r="G58" s="14">
+        <v>0</v>
+      </c>
+      <c r="H58" s="20">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="D59" s="1" t="s">
+    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B59" s="19"/>
+      <c r="C59" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="E59" t="s">
+      <c r="D59" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="F59" s="6">
-        <v>2</v>
-      </c>
-      <c r="H59" s="8">
-        <v>0</v>
-      </c>
-      <c r="I59" s="11">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="60" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="D60" s="1" t="s">
+      <c r="E59" s="11">
+        <v>2</v>
+      </c>
+      <c r="F59" s="19"/>
+      <c r="G59" s="14">
+        <v>0</v>
+      </c>
+      <c r="H59" s="20">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B60" s="19"/>
+      <c r="C60" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="E60" t="s">
+      <c r="D60" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="F60" s="6">
+      <c r="E60" s="11">
         <v>4</v>
       </c>
-      <c r="H60" s="8">
-        <v>0</v>
-      </c>
-      <c r="I60" s="11">
+      <c r="F60" s="19"/>
+      <c r="G60" s="14">
+        <v>0</v>
+      </c>
+      <c r="H60" s="20">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
-    <row r="61" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="D61" s="1" t="s">
+    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B61" s="19"/>
+      <c r="C61" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="E61" t="s">
+      <c r="D61" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="F61" s="6">
+      <c r="E61" s="11">
         <v>4</v>
       </c>
-      <c r="H61" s="8">
-        <v>0</v>
-      </c>
-      <c r="I61" s="11">
+      <c r="F61" s="19"/>
+      <c r="G61" s="14">
+        <v>0</v>
+      </c>
+      <c r="H61" s="20">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
-    <row r="62" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="D62" s="1" t="s">
+    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B62" s="19"/>
+      <c r="C62" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="E62" t="s">
+      <c r="D62" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="F62" s="6">
-        <v>2</v>
-      </c>
-      <c r="H62" s="8">
-        <v>0</v>
-      </c>
-      <c r="I62" s="11">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="63" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="D63" s="1" t="s">
+      <c r="E62" s="11">
+        <v>2</v>
+      </c>
+      <c r="F62" s="19"/>
+      <c r="G62" s="14">
+        <v>0</v>
+      </c>
+      <c r="H62" s="20">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B63" s="19"/>
+      <c r="C63" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="E63" t="s">
-        <v>56</v>
-      </c>
-      <c r="F63" s="6">
-        <v>2</v>
-      </c>
-      <c r="H63" s="8">
-        <v>0</v>
-      </c>
-      <c r="I63" s="11">
-        <f t="shared" si="0"/>
-        <v>2</v>
+      <c r="D63" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="E63" s="11">
+        <v>2</v>
+      </c>
+      <c r="F63" s="19"/>
+      <c r="G63" s="14">
+        <v>0.6</v>
+      </c>
+      <c r="H63" s="20">
+        <f t="shared" si="0"/>
+        <v>0.8</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="71" fitToHeight="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>